<commit_message>
now the wet blue split can now process the xlsx
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/TH.xlsx
+++ b/invoice_gen/TEMPLATE/TH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6571AF-F68E-4244-9C15-9C121E75A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C0603-8D50-49ED-9C1C-5EDFDB9CD8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
   </si>
@@ -466,9 +466,6 @@
   </si>
   <si>
     <t>[[NET]]</t>
-  </si>
-  <si>
-    <t>[[PRICE]]</t>
   </si>
   <si>
     <t>[[AMOUNT]]</t>
@@ -1247,12 +1244,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="169" fontId="30" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,11 +1268,17 @@
     <xf numFmtId="169" fontId="31" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1289,24 +1298,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1318,21 +1330,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1620,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD23B12-9929-48FA-9185-DC4087216413}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1637,15 +1634,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="68" customFormat="1" ht="45.95" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
     </row>
     <row r="2" spans="1:7" s="70" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="69"/>
@@ -1665,7 +1662,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="70" customFormat="1" ht="30" customHeight="1">
@@ -1800,15 +1797,15 @@
       <c r="G16" s="79"/>
     </row>
     <row r="17" spans="1:8" s="76" customFormat="1" ht="54.95" customHeight="1">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
     </row>
     <row r="18" spans="1:8" s="68" customFormat="1" ht="15.75">
       <c r="A18" s="80"/>
@@ -1859,19 +1856,19 @@
         <v>75</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="68" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A21" s="106"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="108" t="s">
+      <c r="A21" s="108"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="109"/>
+      <c r="D21" s="111"/>
       <c r="E21" s="83">
         <f>SUM(E20:E20)</f>
         <v>0</v>
@@ -1937,11 +1934,11 @@
       <c r="B26" s="80"/>
       <c r="C26" s="80"/>
       <c r="D26" s="80"/>
-      <c r="E26" s="105" t="s">
+      <c r="E26" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
     </row>
     <row r="27" spans="1:8" s="76" customFormat="1" ht="41.1" customHeight="1">
       <c r="A27" s="80" t="s">
@@ -1950,11 +1947,11 @@
       <c r="B27" s="80"/>
       <c r="C27" s="80"/>
       <c r="D27" s="80"/>
-      <c r="E27" s="105" t="s">
+      <c r="E27" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
     </row>
     <row r="28" spans="1:8" s="76" customFormat="1" ht="29.1" customHeight="1">
       <c r="A28" s="80" t="s">
@@ -1963,11 +1960,11 @@
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
       <c r="D28" s="80"/>
-      <c r="E28" s="110" t="s">
+      <c r="E28" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
+      <c r="F28" s="105"/>
+      <c r="G28" s="105"/>
     </row>
     <row r="29" spans="1:8" s="76" customFormat="1" ht="29.1" customHeight="1">
       <c r="A29" s="80" t="s">
@@ -2001,17 +1998,17 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="76" customFormat="1" ht="57" customHeight="1">
-      <c r="A32" s="111" t="s">
+      <c r="A32" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="111"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="87"/>
       <c r="D32" s="87"/>
       <c r="E32" s="79"/>
-      <c r="F32" s="111" t="s">
+      <c r="F32" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="111"/>
+      <c r="G32" s="106"/>
     </row>
     <row r="33" s="76" customFormat="1" ht="27.95" customHeight="1"/>
     <row r="34" s="68" customFormat="1" ht="32.1" customHeight="1"/>
@@ -2038,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -2060,70 +2057,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
     </row>
     <row r="3" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
     </row>
     <row r="6" spans="1:11" ht="39.950000000000003" customHeight="1">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="114"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
     </row>
     <row r="7" spans="1:11" ht="21.95" customHeight="1">
       <c r="A7" s="6"/>
@@ -2135,7 +2132,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="27.75" customHeight="1">
@@ -2167,7 +2164,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="22.5" customHeight="1">
@@ -2355,17 +2352,17 @@
         <v>75</v>
       </c>
       <c r="F22" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="38" t="s">
         <v>76</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>77</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:12" ht="27.75" customHeight="1">
       <c r="A23" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="40"/>
       <c r="D23" s="41"/>
@@ -2403,10 +2400,10 @@
     </row>
     <row r="26" spans="1:12" ht="27.75" customHeight="1">
       <c r="A26" s="50"/>
-      <c r="B26" s="113" t="s">
+      <c r="B26" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="113"/>
+      <c r="C26" s="117"/>
       <c r="D26" s="41"/>
       <c r="E26" s="49"/>
       <c r="G26" s="41"/>
@@ -2416,8 +2413,8 @@
     </row>
     <row r="27" spans="1:12" ht="27.75" customHeight="1">
       <c r="A27" s="51"/>
-      <c r="B27" s="113"/>
-      <c r="C27" s="113"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
       <c r="D27" s="41"/>
       <c r="E27" s="52"/>
       <c r="F27" s="43"/>
@@ -2429,7 +2426,7 @@
         <v>35</v>
       </c>
       <c r="C28" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="57">
@@ -2452,11 +2449,11 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:12" ht="42" customHeight="1">
-      <c r="A30" s="115" t="s">
+      <c r="A30" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="115"/>
-      <c r="C30" s="115"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
       <c r="D30" s="60"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
@@ -2466,47 +2463,47 @@
       <c r="A31" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="116" t="s">
+      <c r="B31" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="116"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="62"/>
       <c r="E31" s="62"/>
       <c r="F31" s="18"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="56.1" customHeight="1">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="121"/>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="63"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="112"/>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="116"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A34" s="112" t="s">
+      <c r="A34" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="112"/>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
     </row>
     <row r="35" spans="1:7" ht="45" customHeight="1">
       <c r="A35" s="1"/>
@@ -2589,11 +2586,6 @@
     <row r="70" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="A6:G6"/>
@@ -2601,6 +2593,11 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J30:J42">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2615,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD5BC29-8642-405F-9E90-D798D9601901}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2633,82 +2630,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="54" customHeight="1">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -2722,7 +2719,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1">
@@ -2758,7 +2755,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" ht="22.5" customHeight="1">
@@ -2777,7 +2774,7 @@
       <c r="I10" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="124"/>
+      <c r="N10" s="129"/>
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1">
       <c r="A11" s="29"/>
@@ -2789,7 +2786,7 @@
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="90"/>
-      <c r="N11" s="124"/>
+      <c r="N11" s="129"/>
     </row>
     <row r="12" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="A12" s="27" t="s">
@@ -2805,7 +2802,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="90"/>
-      <c r="N12" s="124"/>
+      <c r="N12" s="129"/>
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="A13" s="29"/>
@@ -2819,7 +2816,7 @@
       <c r="G13" s="92"/>
       <c r="H13" s="92"/>
       <c r="I13" s="90"/>
-      <c r="N13" s="124"/>
+      <c r="N13" s="129"/>
     </row>
     <row r="14" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A14" s="29"/>
@@ -2833,7 +2830,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="90"/>
-      <c r="N14" s="124"/>
+      <c r="N14" s="129"/>
     </row>
     <row r="15" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A15" s="29"/>
@@ -2847,7 +2844,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="90"/>
-      <c r="N15" s="124"/>
+      <c r="N15" s="129"/>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A16" s="9" t="s">
@@ -2863,7 +2860,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="90"/>
-      <c r="N16" s="124"/>
+      <c r="N16" s="129"/>
     </row>
     <row r="17" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A17" s="29"/>
@@ -2877,7 +2874,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="90"/>
-      <c r="N17" s="124"/>
+      <c r="N17" s="129"/>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A18" s="29"/>
@@ -2891,7 +2888,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="90"/>
-      <c r="N18" s="124"/>
+      <c r="N18" s="129"/>
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="24"/>
@@ -2903,7 +2900,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="90"/>
-      <c r="N19" s="124"/>
+      <c r="N19" s="129"/>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A20" s="93" t="s">
@@ -2919,7 +2916,7 @@
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="90"/>
-      <c r="N20" s="124"/>
+      <c r="N20" s="129"/>
     </row>
     <row r="21" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A21" s="93"/>
@@ -2931,7 +2928,7 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="90"/>
-      <c r="N21" s="124"/>
+      <c r="N21" s="129"/>
     </row>
     <row r="22" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A22" s="94"/>
@@ -2943,14 +2940,14 @@
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="90"/>
-      <c r="N22" s="124"/>
+      <c r="N22" s="129"/>
     </row>
     <row r="23" spans="1:14" s="3" customFormat="1" ht="42" customHeight="1">
-      <c r="A23" s="125" t="s">
+      <c r="A23" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="125"/>
-      <c r="C23" s="125"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="95"/>
       <c r="E23" s="95"/>
       <c r="F23" s="95"/>
@@ -2962,10 +2959,10 @@
       <c r="A24" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="126" t="s">
+      <c r="B24" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="126"/>
+      <c r="C24" s="131"/>
       <c r="D24" s="98"/>
       <c r="E24" s="98"/>
       <c r="F24" s="98"/>
@@ -2974,11 +2971,11 @@
       <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:14" s="3" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A25" s="127" t="s">
+      <c r="A25" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="127"/>
-      <c r="C25" s="127"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="100"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -2987,30 +2984,30 @@
       <c r="I25" s="90"/>
     </row>
     <row r="26" spans="1:14" s="3" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A26" s="122" t="s">
+      <c r="A26" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="122"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="123"/>
-      <c r="H26" s="123"/>
-      <c r="I26" s="123"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="123"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" ht="42" customHeight="1">
       <c r="A28" s="29"/>
@@ -3044,18 +3041,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="N10:N22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:I26"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="N10:N22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="32" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
working 2 nd layer
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/TH.xlsx
+++ b/invoice_gen/TEMPLATE/TH.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\tools\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C0603-8D50-49ED-9C1C-5EDFDB9CD8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EC04F4-A3D2-4337-A3D9-45E227417627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,6 +1268,24 @@
     <xf numFmtId="169" fontId="31" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1280,31 +1298,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1315,21 +1330,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD23B12-9929-48FA-9185-DC4087216413}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2036,7 +2036,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -2057,70 +2057,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
     </row>
     <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
     </row>
     <row r="3" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
     </row>
     <row r="6" spans="1:11" ht="39.950000000000003" customHeight="1">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
+      <c r="B6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
     </row>
     <row r="7" spans="1:11" ht="21.95" customHeight="1">
       <c r="A7" s="6"/>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="26" spans="1:12" ht="27.75" customHeight="1">
       <c r="A26" s="50"/>
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="117"/>
+      <c r="C26" s="113"/>
       <c r="D26" s="41"/>
       <c r="E26" s="49"/>
       <c r="G26" s="41"/>
@@ -2413,8 +2413,8 @@
     </row>
     <row r="27" spans="1:12" ht="27.75" customHeight="1">
       <c r="A27" s="51"/>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
       <c r="D27" s="41"/>
       <c r="E27" s="52"/>
       <c r="F27" s="43"/>
@@ -2449,11 +2449,11 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:12" ht="42" customHeight="1">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="119"/>
-      <c r="C30" s="119"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="115"/>
       <c r="D30" s="60"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
@@ -2463,47 +2463,47 @@
       <c r="A31" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="120" t="s">
+      <c r="B31" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="120"/>
+      <c r="C31" s="116"/>
       <c r="D31" s="62"/>
       <c r="E31" s="62"/>
       <c r="F31" s="18"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="56.1" customHeight="1">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="121"/>
-      <c r="C32" s="121"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="117"/>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="63"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A34" s="116" t="s">
+      <c r="A34" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
     </row>
     <row r="35" spans="1:7" ht="45" customHeight="1">
       <c r="A35" s="1"/>
@@ -2586,6 +2586,11 @@
     <row r="70" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="A6:G6"/>
@@ -2593,11 +2598,6 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J30:J42">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2630,82 +2630,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="54" customHeight="1">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -2774,7 +2774,7 @@
       <c r="I10" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="129"/>
+      <c r="N10" s="124"/>
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1">
       <c r="A11" s="29"/>
@@ -2786,7 +2786,7 @@
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="90"/>
-      <c r="N11" s="129"/>
+      <c r="N11" s="124"/>
     </row>
     <row r="12" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="A12" s="27" t="s">
@@ -2802,7 +2802,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="90"/>
-      <c r="N12" s="129"/>
+      <c r="N12" s="124"/>
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="A13" s="29"/>
@@ -2816,7 +2816,7 @@
       <c r="G13" s="92"/>
       <c r="H13" s="92"/>
       <c r="I13" s="90"/>
-      <c r="N13" s="129"/>
+      <c r="N13" s="124"/>
     </row>
     <row r="14" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A14" s="29"/>
@@ -2830,7 +2830,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="90"/>
-      <c r="N14" s="129"/>
+      <c r="N14" s="124"/>
     </row>
     <row r="15" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A15" s="29"/>
@@ -2844,7 +2844,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="90"/>
-      <c r="N15" s="129"/>
+      <c r="N15" s="124"/>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A16" s="9" t="s">
@@ -2860,7 +2860,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="90"/>
-      <c r="N16" s="129"/>
+      <c r="N16" s="124"/>
     </row>
     <row r="17" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A17" s="29"/>
@@ -2874,7 +2874,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="90"/>
-      <c r="N17" s="129"/>
+      <c r="N17" s="124"/>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A18" s="29"/>
@@ -2888,7 +2888,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="90"/>
-      <c r="N18" s="129"/>
+      <c r="N18" s="124"/>
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="24"/>
@@ -2900,7 +2900,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="90"/>
-      <c r="N19" s="129"/>
+      <c r="N19" s="124"/>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A20" s="93" t="s">
@@ -2916,7 +2916,7 @@
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="90"/>
-      <c r="N20" s="129"/>
+      <c r="N20" s="124"/>
     </row>
     <row r="21" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A21" s="93"/>
@@ -2928,7 +2928,7 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="90"/>
-      <c r="N21" s="129"/>
+      <c r="N21" s="124"/>
     </row>
     <row r="22" spans="1:14" s="3" customFormat="1" ht="27.75" customHeight="1">
       <c r="A22" s="94"/>
@@ -2940,14 +2940,14 @@
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="90"/>
-      <c r="N22" s="129"/>
+      <c r="N22" s="124"/>
     </row>
     <row r="23" spans="1:14" s="3" customFormat="1" ht="42" customHeight="1">
-      <c r="A23" s="130" t="s">
+      <c r="A23" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="130"/>
-      <c r="C23" s="130"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="125"/>
       <c r="D23" s="95"/>
       <c r="E23" s="95"/>
       <c r="F23" s="95"/>
@@ -2959,10 +2959,10 @@
       <c r="A24" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="131" t="s">
+      <c r="B24" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="131"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="98"/>
       <c r="E24" s="98"/>
       <c r="F24" s="98"/>
@@ -2971,11 +2971,11 @@
       <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:14" s="3" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="127" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
+      <c r="B25" s="127"/>
+      <c r="C25" s="127"/>
       <c r="D25" s="100"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -2984,30 +2984,30 @@
       <c r="I25" s="90"/>
     </row>
     <row r="26" spans="1:14" s="3" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A26" s="128" t="s">
+      <c r="A26" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="124"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="123"/>
+      <c r="H26" s="123"/>
+      <c r="I26" s="123"/>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="128" t="s">
+      <c r="A27" s="122" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="124"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="123"/>
+      <c r="H27" s="123"/>
+      <c r="I27" s="123"/>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" ht="42" customHeight="1">
       <c r="A28" s="29"/>
@@ -3041,18 +3041,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="N10:N22"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="32" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>